<commit_message>
added matrix, matlab var
</commit_message>
<xml_diff>
--- a/Cost matrix.xlsx
+++ b/Cost matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tang-\Documents\Python\skynet2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tang-\Documents\Python Scripts\skynet2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A682B48-C2AF-4DAF-B064-8550EF89F43D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1532FA1-D9EB-43B5-A5D7-A619B5415151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CCA6E2E4-1C14-4D20-99C2-39AF62563567}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{CCA6E2E4-1C14-4D20-99C2-39AF62563567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,10 +28,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,12 +380,12 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="B1">
         <v>0</v>
       </c>
@@ -442,7 +438,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -451,71 +447,71 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:R17" si="0">ABS(C$1-$A2)^2</f>
-        <v>1</v>
+        <f>2*ABS(C$1-$A2)^2</f>
+        <v>2</v>
       </c>
       <c r="D2">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" ref="D2:R2" si="0">2*ABS(D$1-$A2)^2</f>
+        <v>8</v>
       </c>
       <c r="E2">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F2">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H2">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="I2">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="J2">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="K2">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="L2">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="M2">
         <f t="shared" si="0"/>
-        <v>121</v>
+        <v>242</v>
       </c>
       <c r="N2">
         <f t="shared" si="0"/>
-        <v>144</v>
+        <v>288</v>
       </c>
       <c r="O2">
         <f t="shared" si="0"/>
-        <v>196</v>
+        <v>392</v>
       </c>
       <c r="P2">
         <f t="shared" si="0"/>
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="Q2">
         <f t="shared" si="0"/>
-        <v>324</v>
+        <v>648</v>
       </c>
       <c r="R2">
         <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -524,71 +520,71 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C2:R17" si="2">ABS(C$1-$A3)^2</f>
         <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="J3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="L3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="M3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="N3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="O3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="P3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>225</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>289</v>
       </c>
       <c r="R3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>361</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -597,71 +593,71 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>196</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>256</v>
       </c>
       <c r="R4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>324</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -670,71 +666,71 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="L5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="M5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="N5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="O5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="P5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>225</v>
       </c>
       <c r="R5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>289</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -743,71 +739,71 @@
         <v>16</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="L6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="M6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="N6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="O6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="P6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>196</v>
       </c>
       <c r="R6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -816,71 +812,71 @@
         <v>25</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="L7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="M7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="N7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="O7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="P7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="R7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
@@ -889,71 +885,71 @@
         <v>36</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="L8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="M8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="N8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="O8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="P8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="R8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>
@@ -962,71 +958,71 @@
         <v>49</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="M9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="N9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="O9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="P9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="R9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1035,71 +1031,71 @@
         <v>64</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="M10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="N10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="O10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="P10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="R10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1108,71 +1104,71 @@
         <v>81</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="N11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="O11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="P11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="R11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1181,71 +1177,71 @@
         <v>100</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="O12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="P12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="R12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1254,71 +1250,71 @@
         <v>121</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="K13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="P13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="R13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1327,71 +1323,71 @@
         <v>144</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="I14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="J14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="K14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="L14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="M14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="P14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="R14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1400,71 +1396,71 @@
         <v>196</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="I15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="J15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="K15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="L15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="M15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="N15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="O15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="R15">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1473,71 +1469,71 @@
         <v>256</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>225</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>196</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="I16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="J16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="K16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="L16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="M16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="N16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="O16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="P16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="R16">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>18</v>
       </c>
@@ -1546,71 +1542,71 @@
         <v>324</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>289</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>256</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>225</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>196</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="I17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="J17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="K17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="L17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="M17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="N17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="O17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="P17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R17">
-        <f t="shared" ref="C17:R18" si="2">ABS(R$1-$A17)^2</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+        <f t="shared" ref="C17:R18" si="3">ABS(R$1-$A17)^2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>20</v>
       </c>
@@ -1619,67 +1615,67 @@
         <v>400</v>
       </c>
       <c r="C18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>361</v>
       </c>
       <c r="D18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>324</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>289</v>
       </c>
       <c r="F18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>256</v>
       </c>
       <c r="G18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>225</v>
       </c>
       <c r="H18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>196</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>169</v>
       </c>
       <c r="J18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>144</v>
       </c>
       <c r="K18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>121</v>
       </c>
       <c r="L18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="M18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="N18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="O18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="P18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="R18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>